<commit_message>
first commit - TC Highlight
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>KeyOFF
 NBC is in "ACTIVE ALARM" state
@@ -114,6 +114,20 @@
   </si>
   <si>
     <t>PRECONDITIONS</t>
+  </si>
+  <si>
+    <t>Key OFF
+Alarm armed
+NBC::[C1].STATUS_B_CAN.TheftAlarmStatus=0x2("VTA_ARM")
+Deterring LED blinking with frequency 1 Hz duty-cycle 8%
+MUW is powered ON
+ON LIN, the schedule "Sleep Armed" is running
+NBC programmed_x000D_
+EOL:_x000D_
+"AlarmSystem"(Byte:64;Bit:0)=0x1("Present")_x000D_
+"Siren"(Byte:65;Bit:0)=0x1("Present")_x000D_
+"Side driver"(Byte 58;Bit 4)=0x1("right")_x000D_
+"Country Code"(Byte 64;Bit 4-7)=0x2("UK")</t>
   </si>
 </sst>
 </file>
@@ -495,93 +509,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="82.77734375" customWidth="1"/>
     <col min="2" max="2" width="97" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
@@ -596,27 +612,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>